<commit_message>
Optimize matrix multiplication with block access of elements
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/MulTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/MulTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19440" windowHeight="11040" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19440" windowHeight="11040" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="5x5 mul 5x5" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="13x1 mul 1x4" sheetId="6" r:id="rId5"/>
     <sheet name="Scalar mul 7x7" sheetId="7" r:id="rId6"/>
     <sheet name="Scalar mul 13x2" sheetId="8" r:id="rId7"/>
-    <sheet name="rand" sheetId="3" r:id="rId8"/>
+    <sheet name="8x4 mul 4x8" sheetId="9" r:id="rId8"/>
+    <sheet name="rand" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
   <si>
     <t>#0</t>
   </si>
@@ -2434,7 +2435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:B35"/>
     </sheetView>
   </sheetViews>
@@ -2725,10 +2726,489 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>16.988893341023498</v>
+      </c>
+      <c r="B3">
+        <v>-6.1006649232955077</v>
+      </c>
+      <c r="C3">
+        <v>5.5798583655997724</v>
+      </c>
+      <c r="D3">
+        <v>-5.3433421507157952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-0.77777326204735431</v>
+      </c>
+      <c r="B4">
+        <v>-5.4406992673412162</v>
+      </c>
+      <c r="C4">
+        <v>22.19493797638885</v>
+      </c>
+      <c r="D4">
+        <v>-9.6945007766385807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15.676891056444759</v>
+      </c>
+      <c r="B5">
+        <v>-20.679389816346529</v>
+      </c>
+      <c r="C5">
+        <v>-16.339318313538641</v>
+      </c>
+      <c r="D5">
+        <v>-9.6768047498527743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-18.120914953738083</v>
+      </c>
+      <c r="B6">
+        <v>-9.2621427071752809</v>
+      </c>
+      <c r="C6">
+        <v>10.803453624205432</v>
+      </c>
+      <c r="D6">
+        <v>-11.58944318427495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.6239593603671665</v>
+      </c>
+      <c r="B7">
+        <v>20.304094778951821</v>
+      </c>
+      <c r="C7">
+        <v>-12.317995864276499</v>
+      </c>
+      <c r="D7">
+        <v>11.264107000914116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>21.524224812462442</v>
+      </c>
+      <c r="B8">
+        <v>-13.744536098890258</v>
+      </c>
+      <c r="C8">
+        <v>20.827715885888118</v>
+      </c>
+      <c r="D8">
+        <v>0.40941068582671036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14.263011089570995</v>
+      </c>
+      <c r="B9">
+        <v>18.235009801707179</v>
+      </c>
+      <c r="C9">
+        <v>-15.267437981903942</v>
+      </c>
+      <c r="D9">
+        <v>4.6039667045529136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-13.409403756069066</v>
+      </c>
+      <c r="B10">
+        <v>5.2572155694703788</v>
+      </c>
+      <c r="C10">
+        <v>-8.2865913032991578</v>
+      </c>
+      <c r="D10">
+        <v>-0.96663715088328672</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17.955385791689778</v>
+      </c>
+      <c r="B14">
+        <v>20.417861941023283</v>
+      </c>
+      <c r="C14">
+        <v>-12.400036741435249</v>
+      </c>
+      <c r="D14">
+        <v>-23.601958007037794</v>
+      </c>
+      <c r="E14">
+        <v>16.644105354965426</v>
+      </c>
+      <c r="F14">
+        <v>4.0733312769421204</v>
+      </c>
+      <c r="G14">
+        <v>-18.270609185199238</v>
+      </c>
+      <c r="H14">
+        <v>-10.661830647187703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>19.630598616990795</v>
+      </c>
+      <c r="B15">
+        <v>13.937794764199232</v>
+      </c>
+      <c r="C15">
+        <v>8.3326190261089863</v>
+      </c>
+      <c r="D15">
+        <v>-8.4058800317304936</v>
+      </c>
+      <c r="E15">
+        <v>10.671802586138398</v>
+      </c>
+      <c r="F15">
+        <v>9.6630997855809255</v>
+      </c>
+      <c r="G15">
+        <v>-7.542468840007178</v>
+      </c>
+      <c r="H15">
+        <v>20.801531043288222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-8.0317015819712623E-2</v>
+      </c>
+      <c r="B16">
+        <v>-21.098336283647022</v>
+      </c>
+      <c r="C16">
+        <v>-14.851233446647999</v>
+      </c>
+      <c r="D16">
+        <v>17.900454069328497</v>
+      </c>
+      <c r="E16">
+        <v>15.74144467803977</v>
+      </c>
+      <c r="F16">
+        <v>19.757036026407484</v>
+      </c>
+      <c r="G16">
+        <v>-23.367698511472728</v>
+      </c>
+      <c r="H16">
+        <v>16.332985961229305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3.2240092893244992</v>
+      </c>
+      <c r="B17">
+        <v>-18.3099490018731</v>
+      </c>
+      <c r="C17">
+        <v>1.0041026708517151</v>
+      </c>
+      <c r="D17">
+        <v>5.2398746585144771</v>
+      </c>
+      <c r="E17">
+        <v>20.681263129997447</v>
+      </c>
+      <c r="F17">
+        <v>-9.2105428042977326</v>
+      </c>
+      <c r="G17">
+        <v>5.2679106214173004</v>
+      </c>
+      <c r="H17">
+        <v>18.921218130997154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="array" ref="A21:H28">MMULT(A3:D10,A14:H17)</f>
+        <v>167.60728740340883</v>
+      </c>
+      <c r="B21">
+        <v>241.95765720836562</v>
+      </c>
+      <c r="C21">
+        <v>-349.73046154834617</v>
+      </c>
+      <c r="D21">
+        <v>-277.8061345024031</v>
+      </c>
+      <c r="E21">
+        <v>194.98780568750323</v>
+      </c>
+      <c r="F21">
+        <v>169.70660104300885</v>
+      </c>
+      <c r="G21">
+        <v>-422.92005252926987</v>
+      </c>
+      <c r="H21">
+        <v>-318.00266850301449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-153.80719423526611</v>
+      </c>
+      <c r="B22">
+        <v>-382.48226724950166</v>
+      </c>
+      <c r="C22">
+        <v>-375.0473365481123</v>
+      </c>
+      <c r="D22">
+        <v>410.59233607131864</v>
+      </c>
+      <c r="E22">
+        <v>77.878458184817362</v>
+      </c>
+      <c r="F22">
+        <v>472.05565549459942</v>
+      </c>
+      <c r="G22">
+        <v>-514.46768672634812</v>
+      </c>
+      <c r="H22">
+        <v>74.19545860788017</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-154.34995731326188</v>
+      </c>
+      <c r="B23">
+        <v>553.7777400413205</v>
+      </c>
+      <c r="C23">
+        <v>-133.76497698459067</v>
+      </c>
+      <c r="D23">
+        <v>-539.36331544929976</v>
+      </c>
+      <c r="E23">
+        <v>-417.09155993883405</v>
+      </c>
+      <c r="F23">
+        <v>-369.65771284502381</v>
+      </c>
+      <c r="G23">
+        <v>200.38302529953322</v>
+      </c>
+      <c r="H23">
+        <v>-1047.2741168533335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-545.42159835045788</v>
+      </c>
+      <c r="B24">
+        <v>-514.81696782387348</v>
+      </c>
+      <c r="C24">
+        <v>-24.559497987694609</v>
+      </c>
+      <c r="D24">
+        <v>638.20502996314656</v>
+      </c>
+      <c r="E24">
+        <v>-470.0725325809488</v>
+      </c>
+      <c r="F24">
+        <v>156.87578613419535</v>
+      </c>
+      <c r="G24">
+        <v>87.435579938686288</v>
+      </c>
+      <c r="H24">
+        <v>-42.298348771351016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>465.04528198795037</v>
+      </c>
+      <c r="B25">
+        <v>369.79607826638858</v>
+      </c>
+      <c r="C25">
+        <v>343.29688282745576</v>
+      </c>
+      <c r="D25">
+        <v>-370.47761586305074</v>
+      </c>
+      <c r="E25">
+        <v>282.76355222587063</v>
+      </c>
+      <c r="F25">
+        <v>-144.30020938778779</v>
+      </c>
+      <c r="G25">
+        <v>164.36779353216647</v>
+      </c>
+      <c r="H25">
+        <v>416.98285026556209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>116.30941290872825</v>
+      </c>
+      <c r="B26">
+        <v>-199.01631522608776</v>
+      </c>
+      <c r="C26">
+        <v>-690.33534192677087</v>
+      </c>
+      <c r="D26">
+        <v>-17.508096356766814</v>
+      </c>
+      <c r="E26">
+        <v>547.89795708662894</v>
+      </c>
+      <c r="F26">
+        <v>362.58351276936838</v>
+      </c>
+      <c r="G26">
+        <v>-774.13201092029249</v>
+      </c>
+      <c r="H26">
+        <v>-167.46969403875985</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>630.13149133974173</v>
+      </c>
+      <c r="B27">
+        <v>783.19516059474961</v>
+      </c>
+      <c r="C27">
+        <v>206.44666892684015</v>
+      </c>
+      <c r="D27">
+        <v>-739.08615744811084</v>
+      </c>
+      <c r="E27">
+        <v>286.8798005050395</v>
+      </c>
+      <c r="F27">
+        <v>-109.7396661617998</v>
+      </c>
+      <c r="G27">
+        <v>-17.112721741011427</v>
+      </c>
+      <c r="H27">
+        <v>64.996121771228403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-140.01962185854171</v>
+      </c>
+      <c r="B28">
+        <v>-7.984996066286989</v>
+      </c>
+      <c r="C28">
+        <v>332.17897271183404</v>
+      </c>
+      <c r="D28">
+        <v>118.89785644534776</v>
+      </c>
+      <c r="E28">
+        <v>-317.51775799217904</v>
+      </c>
+      <c r="F28">
+        <v>-158.63517514360083</v>
+      </c>
+      <c r="G28">
+        <v>393.89199996484172</v>
+      </c>
+      <c r="H28">
+        <v>98.692192987949042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B12" sqref="B12:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,1303 +3216,1303 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*50-25</f>
-        <v>13.874709225368456</v>
+        <v>16.90478996370107</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:J16" ca="1" si="0">RAND()*50-25</f>
-        <v>18.006546994418329</v>
+        <v>13.290032129521343</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>23.531395274992455</v>
+        <v>20.700770406412126</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.601955918702988</v>
+        <v>24.653766924235605</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>16.180233215844304</v>
+        <v>12.31927273072597</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>24.962072562265035</v>
+        <v>-4.9528859577384949</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>20.538579044448781</v>
+        <v>14.404892731247173</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.60007733355895</v>
+        <v>19.257871980874242</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.7951078241069247</v>
+        <v>-18.035061581685923</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.180132225059936</v>
+        <v>-18.803549757127531</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:J31" ca="1" si="1">RAND()*50-25</f>
-        <v>2.5615343760979741</v>
+        <v>4.4646714822417337</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.349536923708882</v>
+        <v>-12.079191044925869</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>14.491309847531319</v>
+        <v>-17.497698628386665</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>23.68175534165843</v>
+        <v>8.0785018980965404</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>18.077959739469826</v>
+        <v>-14.472247530639814</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.4455032795312839</v>
+        <v>17.133385970915604</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.213085861348887</v>
+        <v>13.77387241111942</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7552444583428368</v>
+        <v>-11.579775609453351</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.443599655607414</v>
+        <v>9.894717713519384</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.799990667962795</v>
+        <v>-11.574713565536749</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8342089124450496</v>
+        <v>24.475209364335569</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.966952016420993</v>
+        <v>-16.946624272402328</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>16.232578992591115</v>
+        <v>-19.977669617901761</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>22.487624267212801</v>
+        <v>-24.966169448202812</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.143278649106108</v>
+        <v>-21.435225729553501</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7964780279563435</v>
+        <v>24.788978893240845</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.446352097569985</v>
+        <v>6.3692140371242978</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>17.901634966778872</v>
+        <v>24.033410286262793</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.66204160232525</v>
+        <v>8.021284776701485</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.86123684269879774</v>
+        <v>2.2093821531262421</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.655719052180473</v>
+        <v>20.098420613315781</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4025945119910439</v>
+        <v>24.625409561054759</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>23.193652670146072</v>
+        <v>-19.948152061790591</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.858956832207092</v>
+        <v>3.5725613210874805</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>8.404076200476112</v>
+        <v>22.581600112205621</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.626222324352959</v>
+        <v>20.890106717656138</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.6019842570226928</v>
+        <v>-23.5437728447151</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>11.494497108019829</v>
+        <v>10.745030304296165</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6285593530059757</v>
+        <v>7.0361410404428284</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.3511499190981588</v>
+        <v>-5.2541959140749661</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.5129734500366538</v>
+        <v>7.155144595416715</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.870117385531088</v>
+        <v>4.4274224148598869</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>17.364427056118778</v>
+        <v>5.6236363003875915</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>11.231631641982943</v>
+        <v>-11.584981457982252</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.868825588558952</v>
+        <v>13.948259570196939</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55774477748534679</v>
+        <v>20.183577057191854</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.0511875970436861</v>
+        <v>4.1194946994757551</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.583310492737063</v>
+        <v>5.3707733804496662</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-24.157201894872237</v>
+        <v>14.527702147967737</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72825788294906957</v>
+        <v>0.21657751365081879</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.5847387413268308</v>
+        <v>-9.2847367295842869</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.316722679141247</v>
+        <v>-17.062513320246836</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>15.98101472360046</v>
+        <v>-22.812746060544487</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.265285068075833</v>
+        <v>-9.4571684560801224</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8978506959041788</v>
+        <v>-22.290854886555035</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.97535922012228</v>
+        <v>-1.1041607847960648</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.521796343896852</v>
+        <v>7.4939527934918928</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.5076606458693043</v>
+        <v>-3.1531359297065684</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4213435180547975</v>
+        <v>8.9963628760765033</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>-24.360836717488006</v>
+        <v>-14.573675404516646</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.5236471196320274</v>
+        <v>-20.057449824569019</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>14.165257715819735</v>
+        <v>15.437828586073628</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.1196455324706847</v>
+        <v>-17.130209275791685</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.216704114380292</v>
+        <v>-19.728149290324964</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>20.786956560334957</v>
+        <v>15.968128855727137</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>11.644393164868738</v>
+        <v>1.4336984453256534</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6028703306042829</v>
+        <v>14.471767098687785</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.825013014854161</v>
+        <v>-1.1672423674699566</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.930911630978564</v>
+        <v>2.3017782126344137</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9393288450925681</v>
+        <v>18.791427595842769</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>22.677639641523065</v>
+        <v>-22.104998005987831</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.477229892459178</v>
+        <v>-10.512283398199623</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6196415427123156</v>
+        <v>17.758511126727463</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3303567719936318</v>
+        <v>-17.902485916282806</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>20.826289403309787</v>
+        <v>-13.581580314777819</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-14.676877358989875</v>
+        <v>22.031135238585094</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6636709430287908</v>
+        <v>2.5004887160686948</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.266951200793379</v>
+        <v>-21.508699053139036</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2633204628053107</v>
+        <v>-11.670017402022204</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>19.27377321659683</v>
+        <v>-4.6972958569200323</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>18.535931665645869</v>
+        <v>-9.5133714961206586</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>17.917887305250879</v>
+        <v>-9.1702466374482547</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13324986811458217</v>
+        <v>-4.0345431274084191</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.523190230362736</v>
+        <v>-13.112036094469742</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.042448009453683</v>
+        <v>-20.900290296512352</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5134737278046657</v>
+        <v>15.622131032387919</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>20.797701182805042</v>
+        <v>-16.43151277356408</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.393056749464542</v>
+        <v>-19.244077798358756</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9391274149271602</v>
+        <v>-21.891844377554758</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.531641867968542</v>
+        <v>-2.973298822665992</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.2684592302796247</v>
+        <v>-1.9883717171661708</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.966498419707495</v>
+        <v>9.6501424679785117</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>11.172529908642097</v>
+        <v>5.8972614825821985</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3318427202112062</v>
+        <v>9.3558472148259924</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>19.286733047189095</v>
+        <v>-3.4173062809833397</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1516635351798179</v>
+        <v>8.2838774579011201</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5718332585745571</v>
+        <v>3.857438080617122</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>21.53156394399322</v>
+        <v>-3.1740643935103741</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>10.90819186088212</v>
+        <v>-7.6882096556216872</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>23.657883298025062</v>
+        <v>-10.896531068050692</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1487797946991378</v>
+        <v>-6.9138468220015454</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.708274787147467</v>
+        <v>13.701952032245885</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.6504745840792214</v>
+        <v>-5.311837632297145</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>13.216459422843222</v>
+        <v>-18.89421009131642</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9633867046401008</v>
+        <v>-8.2744829101971078</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.092037236628421</v>
+        <v>-23.846288406751793</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>11.383911609198336</v>
+        <v>-5.7986575189565137</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>17.134644768240435</v>
+        <v>3.7921946102786528</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.613728562996972</v>
+        <v>-11.081139120905714</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>-20.825482615952506</v>
+        <v>22.301033417572278</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.961255878588982</v>
+        <v>10.416281525683743</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>13.803656572290194</v>
+        <v>-21.998695806898205</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>18.124133692402133</v>
+        <v>6.4735909266002025</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.831528606765801</v>
+        <v>-6.3057430506943781</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>10.409807284069885</v>
+        <v>-1.0479776595032675</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.943789420411036</v>
+        <v>-19.845627301183004</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.71712032061977</v>
+        <v>-13.6375265011007</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.052799665940686</v>
+        <v>17.721317577276707</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>12.037212441371132</v>
+        <v>-16.253972707020104</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0310826949928611</v>
+        <v>-14.841881920568845</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.334897917123246</v>
+        <v>-23.992873127433423</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>15.987201721282894</v>
+        <v>-22.106877309763323</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-19.612406248806092</v>
+        <v>1.5004481597232342</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76858629957459357</v>
+        <v>-15.45371439194575</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>12.293075566104235</v>
+        <v>-17.48491482624754</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>16.817675166047593</v>
+        <v>13.224166758569226</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.0790148016394383</v>
+        <v>-9.7816987741059229</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-17.902990886210539</v>
+        <v>-23.611334555304136</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>15.804534103174653</v>
+        <v>12.350600109801761</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.954655881800802</v>
+        <v>2.3275158365077537</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>20.705272005888645</v>
+        <v>-8.4000529618235191</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.413681797980232</v>
+        <v>-12.175723186139836</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>16.965125738398676</v>
+        <v>22.883849134836709</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0594821420094114</v>
+        <v>4.4940709489505615</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.847670847019298</v>
+        <v>-20.783600188558708</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>12.106703355214357</v>
+        <v>4.3412439710099733</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2177409663532721</v>
+        <v>0.45201713323342929</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.916907235717453</v>
+        <v>2.4582859021270664</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.885764679671254</v>
+        <v>-9.6649264600358435</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>14.853351540477696</v>
+        <v>-10.702109936963177</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8231144444980494</v>
+        <v>15.669655016579732</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68104622312842267</v>
+        <v>-21.270276504751102</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>15.99436078879701</v>
+        <v>4.1491815559019045</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.4133406058585223</v>
+        <v>11.957974785574521</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>19.505443167539454</v>
+        <v>-7.1224088712752867</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.8926295313376293</v>
+        <v>-4.174865599415579</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.684561954545714</v>
+        <v>-0.98552256490532386</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.333992344297329</v>
+        <v>-18.703467939950595</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.512015452146118</v>
+        <v>-11.132530471493872</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8235841944542059</v>
+        <v>-18.688334570309973</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0913129056079605</v>
+        <v>14.302524377903133</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.960652583599796</v>
+        <v>-1.4400414930930623</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8021293002906873</v>
+        <v>-10.213607048902878</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>-22.218935816859688</v>
+        <v>18.228923951685886</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>16.827990432259341</v>
+        <v>7.3301915218008773</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.65531410775983</v>
+        <v>11.316822340628228</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>13.827334136926645</v>
+        <v>-9.3071481537413838</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9108406074923359</v>
+        <v>-14.964392284512485</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7527513662418635</v>
+        <v>12.215587877632281</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.311931977320507</v>
+        <v>5.1360591082317271</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2005370953963244</v>
+        <v>-24.777551894723356</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2540492837507777</v>
+        <v>-2.874038557852387</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5637305846789857</v>
+        <v>-10.672725706885316</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.671140895129781</v>
+        <v>-0.29307031994871124</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.965169637931579</v>
+        <v>14.784044322368317</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.350713524926013</v>
+        <v>16.785382903287271</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.792988626493717</v>
+        <v>3.9764346877037902</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8428722288760362</v>
+        <v>-11.729684148312186</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.4342457264381459</v>
+        <v>1.9526073593155715</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7264661101637557</v>
+        <v>-18.940800184108369</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>19.559073177982746</v>
+        <v>-16.355902749253879</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.890927953473554</v>
+        <v>15.446090789515928</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>24.539345699947383</v>
+        <v>-18.024624192466348</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.751816900594402</v>
+        <v>-4.3019478168694185</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1836273982916659</v>
+        <v>-17.175577139327729</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.414859362823332</v>
+        <v>-21.230260411706318</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>14.325595212851603</v>
+        <v>-7.2263743997109948</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1549453187683305</v>
+        <v>19.849988620312544</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>22.782112185716933</v>
+        <v>-13.835602220424231</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3224273960957156</v>
+        <v>5.7627595363785424</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>24.539314831351234</v>
+        <v>-8.2170256757868039</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>16.174514395035985</v>
+        <v>18.280599866247151</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.7360633345871701</v>
+        <v>7.9758492693873606</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.091838289248678</v>
+        <v>24.826802234026452</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.556668666417821</v>
+        <v>23.753647949886933</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.943586254501536</v>
+        <v>-16.701145546106751</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.9171399638268518</v>
+        <v>24.968006606982271</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6771857804699977</v>
+        <v>22.836305851762312</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.5274671633343821</v>
+        <v>13.135158968829721</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.679236231490727</v>
+        <v>-4.2772457333855591</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>15.111213145974226</v>
+        <v>4.1603668157072562</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2799492807325308</v>
+        <v>-15.034184580174671</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.356510423567013</v>
+        <v>-7.7004869255438635</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>18.608060868144072</v>
+        <v>-21.755911565833259</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.42356684785898</v>
+        <v>12.936213758162232</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.4669883428449282</v>
+        <v>-7.7198073273399963</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.1922941119858095</v>
+        <v>-10.926638352090151</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3428611594521342</v>
+        <v>-2.4949712326820013</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>23.91973086680008</v>
+        <v>24.249164855197982</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.5865797289960035</v>
+        <v>-17.413977327089192</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>23.571689599959036</v>
+        <v>-13.737653574915893</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.335764719743025</v>
+        <v>17.349357170174386</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5124653498583278</v>
+        <v>-9.6893878041276249</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>14.240131638375317</v>
+        <v>-22.776148560443325</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.869831606856625</v>
+        <v>3.1038370757631384E-2</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.87822320696907</v>
+        <v>21.169897889123988</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.7800575833738641</v>
+        <v>3.2421141427823201</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.5127911703757562</v>
+        <v>-16.011228036106129</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.871154024579841</v>
+        <v>8.7654477552524952</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3384713805702546</v>
+        <v>-12.054207531881961</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.39795363144267171</v>
+        <v>24.084750549094913</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81876267503774969</v>
+        <v>13.650645886094829</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>18.940021993728692</v>
+        <v>-9.466098745997769</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>17.06165118755677</v>
+        <v>-9.1444071580674908</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0791394278660391</v>
+        <v>-10.906536694839652</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.661506050755197</v>
+        <v>-8.4263891470860592</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>21.800006426345959</v>
+        <v>11.485104883801803</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.9707730340048464</v>
+        <v>-14.143793851571223</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.22692412072837</v>
+        <v>-17.468182100746681</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>14.479093750578961</v>
+        <v>20.461006971022577</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.870060169103354</v>
+        <v>4.4667654574213387</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6889027262059422</v>
+        <v>11.560329724673032</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>12.035829137987619</v>
+        <v>-17.808255345032777</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>18.480215919954638</v>
+        <v>1.6424500134961342</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>13.397759169509996</v>
+        <v>22.468247476946246</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>14.731797902916391</v>
+        <v>3.5680880794708649</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>22.009372546572251</v>
+        <v>-9.3318269400536771</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>23.06652070610555</v>
+        <v>7.5774352019200819</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.52863404749046</v>
+        <v>11.215574465184815</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.199056170053634</v>
+        <v>7.3731097598406237</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.0924985815774235</v>
+        <v>-5.4246462307330319</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>14.742925577237287</v>
+        <v>20.793466330860696</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7411481721280886</v>
+        <v>20.586969536258728</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.3098292615550911</v>
+        <v>-8.9432568098189407</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>20.009473782086765</v>
+        <v>-16.125785126314987</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5782951610088745</v>
+        <v>-5.8707666627006212</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.73504510888397</v>
+        <v>-20.067740122079929</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.30676591324469271</v>
+        <v>-18.568169402699212</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.211254397045836</v>
+        <v>-3.6841370969698417</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9245608126714302</v>
+        <v>-13.290124702886663</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>24.115842856683322</v>
+        <v>-0.79776540058303524</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.209568572224363</v>
+        <v>-21.968895959636285</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.304541890879346</v>
+        <v>4.8505079743282593</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>22.235016731361505</v>
+        <v>-8.9618169245798782</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>21.969885535554816</v>
+        <v>-13.097286909018063</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3229829300044358</v>
+        <v>7.5233068797887128</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>18.055685326532</v>
+        <v>13.48855356670515</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.2003016534413469</v>
+        <v>-10.537767192156295</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>12.644779600353708</v>
+        <v>-18.944065312950858</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>18.337691544052298</v>
+        <v>-23.831803810104979</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.3659983221681884</v>
+        <v>-23.268973939230641</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>20.62794169105986</v>
+        <v>8.2144881023700975</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7294306180494239</v>
+        <v>-21.452524356074669</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>19.864414489809555</v>
+        <v>-18.141083018652232</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>20.018579455743968</v>
+        <v>14.57606890610878</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.4752377667307925</v>
+        <v>-23.400823546895943</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.6551632224443829</v>
+        <v>-22.633849893759301</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>12.274701282350819</v>
+        <v>6.8869136929183341</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>20.451156060174597</v>
+        <v>-0.56233689479576299</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.292931126209517</v>
+        <v>-21.785997953961818</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0582337848251804</v>
+        <v>-21.136698413282822</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>17.268387191480095</v>
+        <v>15.277398430024633</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.197726179942073</v>
+        <v>-10.516619795999716</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>4.4567350495811127</v>
+        <v>24.121871863542403</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.838971162918746</v>
+        <v>-19.328459276220155</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0520269206599906</v>
+        <v>20.335468154612983</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.0857334082208219</v>
+        <v>21.881496895209622</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>16.231685383288344</v>
+        <v>-18.832214877266694</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.1940108364467079</v>
+        <v>-24.463821545278552</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.0653557844566492</v>
+        <v>3.3489959299500498</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.274189831861019</v>
+        <v>8.3345949493547522</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>16.01630848218187</v>
+        <v>13.78883579186126</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.8878917381645479</v>
+        <v>-10.680129001240351</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26516027139240705</v>
+        <v>-8.7771534658224724</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3116625618581672</v>
+        <v>7.330299855107441</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.301577855526013</v>
+        <v>-5.2558249583796197</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.435715152435211</v>
+        <v>-3.4059190328275371</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.605932152314015</v>
+        <v>-17.311464230192424</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.042682201315737</v>
+        <v>8.6183133917595924</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>22.902124962269696</v>
+        <v>-5.7683621750475496</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>16.749046482865339</v>
+        <v>-4.5768214419594599</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>12.539826411667434</v>
+        <v>5.3192893816274065</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4177756040469269</v>
+        <v>2.2950414102845862</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.34365237547631</v>
+        <v>-14.620468119684531</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8612783044221359</v>
+        <v>-24.273544584410452</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>17.869411316418606</v>
+        <v>-18.354014226023825</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>20.440006588645602</v>
+        <v>23.601029255621256</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>22.845410776389407</v>
+        <v>-3.1233171697830251</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.459676764994368</v>
+        <v>23.917881532275324</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7697132132234792</v>
+        <v>15.114351161375211</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>14.694988153045607</v>
+        <v>24.129214369009198</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3602327579491664</v>
+        <v>3.8452759421949523</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>16.898064232201484</v>
+        <v>-14.245904598726439</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>14.918938161731575</v>
+        <v>-21.372071460014414</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4739928205310235</v>
+        <v>-16.676792193212712</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>17.215218360174099</v>
+        <v>-12.105583526632602</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>10.906251233139947</v>
+        <v>-15.416673601047282</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.8184112925531153</v>
+        <v>-20.33893269023681</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.699772449526359</v>
+        <v>-19.592297346944932</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.437031604007082</v>
+        <v>-4.869361601648869</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7309649106974661</v>
+        <v>-14.184809038475555</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.2621689963788683</v>
+        <v>10.368550871701018</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.4704184817555479</v>
+        <v>10.683002762723412</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>13.77202449416319</v>
+        <v>17.15330404767596</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>17.100487765707491</v>
+        <v>16.941135518599545</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>11.700442065380628</v>
+        <v>-24.766321050287495</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>13.707765124811679</v>
+        <v>-22.874332162631646</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>-20.082738445342823</v>
+        <v>22.638012528055029</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="1"/>
-        <v>20.512412676748134</v>
+        <v>19.462370887159018</v>
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="1"/>
-        <v>23.040061549585339</v>
+        <v>1.3000916417130917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>